<commit_message>
Upload form ver 1
</commit_message>
<xml_diff>
--- a/DatabaseExcel/NhanVienDaoTao.xlsx
+++ b/DatabaseExcel/NhanVienDaoTao.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>DT001</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>ltkv@gmail.com</t>
+  </si>
+  <si>
+    <t>0352563523</t>
+  </si>
+  <si>
+    <t>0352563524</t>
+  </si>
+  <si>
+    <t>0352563525</t>
+  </si>
+  <si>
+    <t>0352563526</t>
+  </si>
+  <si>
+    <t>0352563527</t>
   </si>
 </sst>
 </file>
@@ -113,9 +128,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -400,14 +416,14 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="35.296875" customWidth="1"/>
     <col min="3" max="3" width="21.296875" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="4" max="4" width="21" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -420,8 +436,8 @@
       <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1">
-        <v>352563523</v>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -434,8 +450,8 @@
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>352563524</v>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -448,8 +464,8 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>352563525</v>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -462,8 +478,8 @@
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
-        <v>352563526</v>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -476,8 +492,8 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5">
-        <v>352563527</v>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -489,5 +505,6 @@
     <hyperlink ref="C5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>